<commit_message>
add more data 6
</commit_message>
<xml_diff>
--- a/data/EastPerth_suburb_properties.xlsx
+++ b/data/EastPerth_suburb_properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DA\Projects\Project3\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Haleh\DA\Projects\Project-3\Project3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{59C80B48-7EB8-44AF-9094-F8AC7F35EAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCD231C-9968-43E2-9A1E-1C7CE221F2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8910" yWindow="4785" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="36015" yWindow="-1695" windowWidth="14625" windowHeight="15765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EastPerth_suburb_properties" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="438">
   <si>
     <t>address</t>
   </si>
@@ -1331,12 +1331,15 @@
   </si>
   <si>
     <t>90/189 Adelaide Terrace</t>
+  </si>
+  <si>
+    <t>Shop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
@@ -2176,22 +2179,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="J239" sqref="J239"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="K301" sqref="K301"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2232,7 +2235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2264,7 +2267,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2299,7 +2302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2331,7 +2334,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2372,7 +2375,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2413,7 +2416,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2454,7 +2457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2495,7 +2498,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2536,7 +2539,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -2577,7 +2580,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2615,7 +2618,7 @@
         <v>41487</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -2656,7 +2659,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -2697,7 +2700,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -2735,7 +2738,7 @@
         <v>43344</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -2770,7 +2773,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2811,7 +2814,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -2852,7 +2855,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -2893,7 +2896,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -2913,7 +2916,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -2951,7 +2954,7 @@
         <v>42461</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -2983,7 +2986,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -3053,7 +3056,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -3094,7 +3097,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -3132,7 +3135,7 @@
         <v>43221</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -3164,7 +3167,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -3205,7 +3208,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -3237,7 +3240,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -3278,7 +3281,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -3316,7 +3319,7 @@
         <v>42614</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -3354,7 +3357,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -3389,7 +3392,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>74</v>
       </c>
@@ -3430,7 +3433,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -3471,7 +3474,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>76</v>
       </c>
@@ -3512,7 +3515,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>432</v>
       </c>
@@ -3547,7 +3550,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>79</v>
       </c>
@@ -3588,7 +3591,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -3623,7 +3626,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -3664,7 +3667,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -3699,7 +3702,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -3740,7 +3743,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>90</v>
       </c>
@@ -3775,7 +3778,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>91</v>
       </c>
@@ -3810,7 +3813,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>92</v>
       </c>
@@ -3845,7 +3848,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -3880,7 +3883,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -3915,7 +3918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -3956,7 +3959,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>98</v>
       </c>
@@ -3988,7 +3991,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -4023,7 +4026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -4055,7 +4058,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -4096,7 +4099,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -4137,7 +4140,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -4172,7 +4175,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>105</v>
       </c>
@@ -4213,7 +4216,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>107</v>
       </c>
@@ -4254,7 +4257,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>109</v>
       </c>
@@ -4286,7 +4289,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>110</v>
       </c>
@@ -4321,7 +4324,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -4362,7 +4365,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>115</v>
       </c>
@@ -4403,7 +4406,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>118</v>
       </c>
@@ -4438,7 +4441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>119</v>
       </c>
@@ -4470,7 +4473,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -4502,7 +4505,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>121</v>
       </c>
@@ -4537,7 +4540,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>122</v>
       </c>
@@ -4572,7 +4575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>123</v>
       </c>
@@ -4607,7 +4610,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>125</v>
       </c>
@@ -4648,7 +4651,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>127</v>
       </c>
@@ -4689,7 +4692,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>129</v>
       </c>
@@ -4730,7 +4733,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>130</v>
       </c>
@@ -4768,7 +4771,7 @@
         <v>43160</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>132</v>
       </c>
@@ -4803,7 +4806,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>134</v>
       </c>
@@ -4838,7 +4841,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>136</v>
       </c>
@@ -4879,7 +4882,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>138</v>
       </c>
@@ -4920,7 +4923,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>139</v>
       </c>
@@ -4958,7 +4961,7 @@
         <v>44228</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>140</v>
       </c>
@@ -4999,7 +5002,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>142</v>
       </c>
@@ -5037,7 +5040,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>143</v>
       </c>
@@ -5069,7 +5072,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>144</v>
       </c>
@@ -5110,7 +5113,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>145</v>
       </c>
@@ -5151,7 +5154,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>146</v>
       </c>
@@ -5189,7 +5192,7 @@
         <v>43374</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>147</v>
       </c>
@@ -5224,7 +5227,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>148</v>
       </c>
@@ -5259,7 +5262,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>149</v>
       </c>
@@ -5294,7 +5297,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>150</v>
       </c>
@@ -5335,7 +5338,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>152</v>
       </c>
@@ -5370,7 +5373,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>153</v>
       </c>
@@ -5405,7 +5408,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>154</v>
       </c>
@@ -5440,7 +5443,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>156</v>
       </c>
@@ -5478,7 +5481,7 @@
         <v>43709</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>157</v>
       </c>
@@ -5519,7 +5522,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>159</v>
       </c>
@@ -5557,7 +5560,7 @@
         <v>44287</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>161</v>
       </c>
@@ -5592,7 +5595,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>162</v>
       </c>
@@ -5624,7 +5627,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>163</v>
       </c>
@@ -5665,7 +5668,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>164</v>
       </c>
@@ -5703,7 +5706,7 @@
         <v>41122</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>166</v>
       </c>
@@ -5735,7 +5738,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>167</v>
       </c>
@@ -5770,7 +5773,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>168</v>
       </c>
@@ -5805,7 +5808,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>169</v>
       </c>
@@ -5843,7 +5846,7 @@
         <v>40817</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>171</v>
       </c>
@@ -5863,7 +5866,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>173</v>
       </c>
@@ -5904,7 +5907,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>175</v>
       </c>
@@ -5945,7 +5948,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>177</v>
       </c>
@@ -5980,7 +5983,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>178</v>
       </c>
@@ -6015,7 +6018,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>179</v>
       </c>
@@ -6056,7 +6059,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>182</v>
       </c>
@@ -6094,7 +6097,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>183</v>
       </c>
@@ -6129,7 +6132,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>185</v>
       </c>
@@ -6161,7 +6164,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>186</v>
       </c>
@@ -6196,7 +6199,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>187</v>
       </c>
@@ -6237,7 +6240,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>190</v>
       </c>
@@ -6272,7 +6275,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>191</v>
       </c>
@@ -6307,7 +6310,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>192</v>
       </c>
@@ -6345,7 +6348,7 @@
         <v>42430</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>193</v>
       </c>
@@ -6380,7 +6383,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>195</v>
       </c>
@@ -6415,7 +6418,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>196</v>
       </c>
@@ -6456,7 +6459,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>198</v>
       </c>
@@ -6491,7 +6494,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>200</v>
       </c>
@@ -6532,7 +6535,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>202</v>
       </c>
@@ -6573,7 +6576,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>205</v>
       </c>
@@ -6611,7 +6614,7 @@
         <v>43983</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>206</v>
       </c>
@@ -6649,7 +6652,7 @@
         <v>43191</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>433</v>
       </c>
@@ -6684,7 +6687,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>207</v>
       </c>
@@ -6725,7 +6728,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>208</v>
       </c>
@@ -6766,7 +6769,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>211</v>
       </c>
@@ -6801,7 +6804,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>212</v>
       </c>
@@ -6839,7 +6842,7 @@
         <v>44136</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>214</v>
       </c>
@@ -6877,7 +6880,7 @@
         <v>42614</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>215</v>
       </c>
@@ -6912,7 +6915,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>216</v>
       </c>
@@ -6944,7 +6947,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>217</v>
       </c>
@@ -6985,7 +6988,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>219</v>
       </c>
@@ -7020,7 +7023,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>434</v>
       </c>
@@ -7055,7 +7058,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>220</v>
       </c>
@@ -7087,7 +7090,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>221</v>
       </c>
@@ -7128,7 +7131,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>222</v>
       </c>
@@ -7169,7 +7172,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>224</v>
       </c>
@@ -7210,7 +7213,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>226</v>
       </c>
@@ -7245,7 +7248,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>227</v>
       </c>
@@ -7280,7 +7283,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>228</v>
       </c>
@@ -7321,7 +7324,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>230</v>
       </c>
@@ -7356,7 +7359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>231</v>
       </c>
@@ -7394,7 +7397,7 @@
         <v>40087</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>233</v>
       </c>
@@ -7435,7 +7438,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>235</v>
       </c>
@@ -7476,7 +7479,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>237</v>
       </c>
@@ -7511,7 +7514,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>238</v>
       </c>
@@ -7552,7 +7555,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>240</v>
       </c>
@@ -7593,7 +7596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>241</v>
       </c>
@@ -7631,7 +7634,7 @@
         <v>43221</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>243</v>
       </c>
@@ -7666,7 +7669,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>245</v>
       </c>
@@ -7707,7 +7710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>247</v>
       </c>
@@ -7742,7 +7745,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>248</v>
       </c>
@@ -7774,7 +7777,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>249</v>
       </c>
@@ -7815,7 +7818,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>250</v>
       </c>
@@ -7850,7 +7853,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>251</v>
       </c>
@@ -7891,7 +7894,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>252</v>
       </c>
@@ -7932,7 +7935,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>253</v>
       </c>
@@ -7973,7 +7976,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>255</v>
       </c>
@@ -8008,7 +8011,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>256</v>
       </c>
@@ -8043,7 +8046,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>257</v>
       </c>
@@ -8084,7 +8087,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>258</v>
       </c>
@@ -8119,7 +8122,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>259</v>
       </c>
@@ -8157,7 +8160,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>261</v>
       </c>
@@ -8198,7 +8201,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>262</v>
       </c>
@@ -8236,7 +8239,7 @@
         <v>42948</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>263</v>
       </c>
@@ -8277,7 +8280,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>264</v>
       </c>
@@ -8315,7 +8318,7 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>266</v>
       </c>
@@ -8347,7 +8350,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>267</v>
       </c>
@@ -8385,7 +8388,7 @@
         <v>43709</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>268</v>
       </c>
@@ -8417,7 +8420,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>269</v>
       </c>
@@ -8455,7 +8458,7 @@
         <v>41275</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>270</v>
       </c>
@@ -8487,7 +8490,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>271</v>
       </c>
@@ -8525,7 +8528,7 @@
         <v>43952</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>272</v>
       </c>
@@ -8563,7 +8566,7 @@
         <v>43556</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>273</v>
       </c>
@@ -8595,7 +8598,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>274</v>
       </c>
@@ -8633,7 +8636,7 @@
         <v>44136</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>275</v>
       </c>
@@ -8665,7 +8668,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>276</v>
       </c>
@@ -8703,7 +8706,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>277</v>
       </c>
@@ -8735,7 +8738,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>435</v>
       </c>
@@ -8767,7 +8770,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>278</v>
       </c>
@@ -8805,7 +8808,7 @@
         <v>41883</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>279</v>
       </c>
@@ -8843,7 +8846,7 @@
         <v>44044</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>280</v>
       </c>
@@ -8881,7 +8884,7 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>281</v>
       </c>
@@ -8919,7 +8922,7 @@
         <v>42339</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>282</v>
       </c>
@@ -8957,7 +8960,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>283</v>
       </c>
@@ -8989,7 +8992,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>284</v>
       </c>
@@ -9027,7 +9030,7 @@
         <v>43101</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>285</v>
       </c>
@@ -9065,7 +9068,7 @@
         <v>44166</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>286</v>
       </c>
@@ -9097,7 +9100,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>287</v>
       </c>
@@ -9135,7 +9138,7 @@
         <v>42186</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>288</v>
       </c>
@@ -9173,7 +9176,7 @@
         <v>44013</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>290</v>
       </c>
@@ -9211,7 +9214,7 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>292</v>
       </c>
@@ -9249,7 +9252,7 @@
         <v>39326</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>293</v>
       </c>
@@ -9284,7 +9287,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>294</v>
       </c>
@@ -9316,7 +9319,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>295</v>
       </c>
@@ -9354,7 +9357,7 @@
         <v>44136</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>296</v>
       </c>
@@ -9392,7 +9395,7 @@
         <v>43313</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>297</v>
       </c>
@@ -9424,7 +9427,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>298</v>
       </c>
@@ -9462,7 +9465,7 @@
         <v>44013</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>299</v>
       </c>
@@ -9500,7 +9503,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>301</v>
       </c>
@@ -9538,7 +9541,7 @@
         <v>43586</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>303</v>
       </c>
@@ -9579,7 +9582,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>305</v>
       </c>
@@ -9617,7 +9620,7 @@
         <v>40940</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>306</v>
       </c>
@@ -9655,7 +9658,7 @@
         <v>43709</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>307</v>
       </c>
@@ -9687,7 +9690,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>308</v>
       </c>
@@ -9725,7 +9728,7 @@
         <v>44105</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>309</v>
       </c>
@@ -9763,7 +9766,7 @@
         <v>44044</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>311</v>
       </c>
@@ -9801,7 +9804,7 @@
         <v>43556</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>312</v>
       </c>
@@ -9842,7 +9845,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>313</v>
       </c>
@@ -9880,7 +9883,7 @@
         <v>42826</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>314</v>
       </c>
@@ -9918,7 +9921,7 @@
         <v>43525</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>315</v>
       </c>
@@ -9950,7 +9953,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>316</v>
       </c>
@@ -9988,7 +9991,7 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>317</v>
       </c>
@@ -10026,7 +10029,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>319</v>
       </c>
@@ -10064,7 +10067,7 @@
         <v>43466</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>321</v>
       </c>
@@ -10102,7 +10105,7 @@
         <v>43983</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>322</v>
       </c>
@@ -10140,7 +10143,7 @@
         <v>44075</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>323</v>
       </c>
@@ -10172,7 +10175,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>324</v>
       </c>
@@ -10210,7 +10213,7 @@
         <v>44105</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>326</v>
       </c>
@@ -10227,7 +10230,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>327</v>
       </c>
@@ -10268,7 +10271,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>328</v>
       </c>
@@ -10303,7 +10306,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>330</v>
       </c>
@@ -10341,7 +10344,7 @@
         <v>43009</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>331</v>
       </c>
@@ -10376,7 +10379,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>332</v>
       </c>
@@ -10405,7 +10408,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>335</v>
       </c>
@@ -10443,7 +10446,7 @@
         <v>43435</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>336</v>
       </c>
@@ -10484,7 +10487,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>436</v>
       </c>
@@ -10516,7 +10519,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>337</v>
       </c>
@@ -10548,7 +10551,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>338</v>
       </c>
@@ -10580,7 +10583,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>339</v>
       </c>
@@ -10618,7 +10621,7 @@
         <v>43983</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>341</v>
       </c>
@@ -10653,7 +10656,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>342</v>
       </c>
@@ -10685,7 +10688,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>343</v>
       </c>
@@ -10717,7 +10720,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>344</v>
       </c>
@@ -10755,7 +10758,7 @@
         <v>43525</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>346</v>
       </c>
@@ -10790,7 +10793,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>347</v>
       </c>
@@ -10822,7 +10825,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>348</v>
       </c>
@@ -10860,7 +10863,7 @@
         <v>41275</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>349</v>
       </c>
@@ -10898,7 +10901,7 @@
         <v>44044</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>350</v>
       </c>
@@ -10930,7 +10933,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>351</v>
       </c>
@@ -10962,7 +10965,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>352</v>
       </c>
@@ -11000,7 +11003,7 @@
         <v>41852</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>353</v>
       </c>
@@ -11023,10 +11026,13 @@
         <v>1</v>
       </c>
       <c r="H240" s="3">
-        <v>4019</v>
+        <v>121</v>
       </c>
       <c r="I240">
-        <v>120</v>
+        <v>94</v>
+      </c>
+      <c r="J240">
+        <v>2000</v>
       </c>
       <c r="K240" t="s">
         <v>89</v>
@@ -11035,7 +11041,7 @@
         <v>40695</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>354</v>
       </c>
@@ -11060,6 +11066,12 @@
       <c r="H241">
         <v>83</v>
       </c>
+      <c r="I241">
+        <v>51</v>
+      </c>
+      <c r="J241">
+        <v>2015</v>
+      </c>
       <c r="K241" t="s">
         <v>70</v>
       </c>
@@ -11067,7 +11079,7 @@
         <v>42156</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>355</v>
       </c>
@@ -11089,6 +11101,15 @@
       <c r="G242">
         <v>1</v>
       </c>
+      <c r="H242" s="3">
+        <v>80</v>
+      </c>
+      <c r="I242">
+        <v>47</v>
+      </c>
+      <c r="J242">
+        <v>2019</v>
+      </c>
       <c r="K242" t="s">
         <v>48</v>
       </c>
@@ -11096,7 +11117,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>356</v>
       </c>
@@ -11131,7 +11152,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>360</v>
       </c>
@@ -11153,8 +11174,17 @@
       <c r="G244">
         <v>1</v>
       </c>
-    </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H244" s="3">
+        <v>113</v>
+      </c>
+      <c r="I244">
+        <v>80</v>
+      </c>
+      <c r="J244">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>361</v>
       </c>
@@ -11164,8 +11194,26 @@
       <c r="C245" s="2">
         <v>44075</v>
       </c>
+      <c r="D245" t="s">
+        <v>13</v>
+      </c>
+      <c r="E245">
+        <v>1</v>
+      </c>
+      <c r="F245">
+        <v>1</v>
+      </c>
+      <c r="G245">
+        <v>1</v>
+      </c>
       <c r="H245" s="3">
-        <v>4481</v>
+        <v>66</v>
+      </c>
+      <c r="I245">
+        <v>40</v>
+      </c>
+      <c r="J245">
+        <v>2011</v>
       </c>
       <c r="K245" t="s">
         <v>362</v>
@@ -11174,7 +11222,7 @@
         <v>43800</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>363</v>
       </c>
@@ -11197,10 +11245,13 @@
         <v>1</v>
       </c>
       <c r="H246" s="3">
-        <v>1839</v>
+        <v>123</v>
       </c>
       <c r="I246">
-        <v>84</v>
+        <v>79</v>
+      </c>
+      <c r="J246">
+        <v>2009</v>
       </c>
       <c r="K246" t="s">
         <v>38</v>
@@ -11209,7 +11260,7 @@
         <v>43374</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>364</v>
       </c>
@@ -11219,9 +11270,27 @@
       <c r="C247" s="2">
         <v>44044</v>
       </c>
+      <c r="D247" t="s">
+        <v>13</v>
+      </c>
+      <c r="E247">
+        <v>2</v>
+      </c>
+      <c r="F247">
+        <v>2</v>
+      </c>
+      <c r="G247">
+        <v>1</v>
+      </c>
       <c r="H247">
         <v>122</v>
       </c>
+      <c r="I247">
+        <v>79</v>
+      </c>
+      <c r="J247">
+        <v>2009</v>
+      </c>
       <c r="K247" t="s">
         <v>21</v>
       </c>
@@ -11229,7 +11298,7 @@
         <v>44013</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>365</v>
       </c>
@@ -11243,19 +11312,22 @@
         <v>17</v>
       </c>
       <c r="E248">
+        <v>4</v>
+      </c>
+      <c r="F248">
+        <v>2</v>
+      </c>
+      <c r="G248">
         <v>3</v>
-      </c>
-      <c r="F248">
-        <v>3</v>
-      </c>
-      <c r="G248">
-        <v>2</v>
       </c>
       <c r="H248">
         <v>234</v>
       </c>
       <c r="I248">
-        <v>264</v>
+        <v>250</v>
+      </c>
+      <c r="J248">
+        <v>2002</v>
       </c>
       <c r="K248" t="s">
         <v>78</v>
@@ -11264,7 +11336,7 @@
         <v>40909</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>366</v>
       </c>
@@ -11287,13 +11359,16 @@
         <v>1</v>
       </c>
       <c r="H249" s="3">
-        <v>1871</v>
+        <v>129</v>
       </c>
       <c r="I249">
         <v>98</v>
       </c>
-    </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J249">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>367</v>
       </c>
@@ -11321,6 +11396,9 @@
       <c r="I250">
         <v>130</v>
       </c>
+      <c r="J250">
+        <v>1996</v>
+      </c>
       <c r="K250" t="s">
         <v>368</v>
       </c>
@@ -11331,7 +11409,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>369</v>
       </c>
@@ -11354,16 +11432,19 @@
         <v>2</v>
       </c>
       <c r="H251" s="3">
-        <v>2501</v>
+        <v>123</v>
       </c>
       <c r="I251">
         <v>123</v>
       </c>
+      <c r="J251">
+        <v>1998</v>
+      </c>
       <c r="M251" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>370</v>
       </c>
@@ -11386,7 +11467,13 @@
         <v>2</v>
       </c>
       <c r="H252">
+        <v>246</v>
+      </c>
+      <c r="I252">
         <v>145</v>
+      </c>
+      <c r="J252">
+        <v>2015</v>
       </c>
       <c r="K252" t="s">
         <v>371</v>
@@ -11395,7 +11482,7 @@
         <v>43525</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>372</v>
       </c>
@@ -11423,8 +11510,11 @@
       <c r="I253">
         <v>75</v>
       </c>
-    </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J253">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>373</v>
       </c>
@@ -11434,12 +11524,27 @@
       <c r="C254" s="2">
         <v>44044</v>
       </c>
+      <c r="D254" t="s">
+        <v>13</v>
+      </c>
+      <c r="E254">
+        <v>4</v>
+      </c>
+      <c r="F254">
+        <v>3</v>
+      </c>
+      <c r="G254">
+        <v>3</v>
+      </c>
       <c r="H254">
         <v>328</v>
       </c>
       <c r="I254">
         <v>232</v>
       </c>
+      <c r="J254">
+        <v>1999</v>
+      </c>
       <c r="K254" t="s">
         <v>374</v>
       </c>
@@ -11447,7 +11552,7 @@
         <v>42826</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>375</v>
       </c>
@@ -11460,8 +11565,26 @@
       <c r="D255" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E255">
+        <v>1</v>
+      </c>
+      <c r="F255">
+        <v>1</v>
+      </c>
+      <c r="G255">
+        <v>1</v>
+      </c>
+      <c r="H255">
+        <v>90</v>
+      </c>
+      <c r="I255">
+        <v>66</v>
+      </c>
+      <c r="J255">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>376</v>
       </c>
@@ -11484,11 +11607,14 @@
         <v>1</v>
       </c>
       <c r="H256" s="3">
-        <v>4019</v>
+        <v>106</v>
       </c>
       <c r="I256">
         <v>79</v>
       </c>
+      <c r="J256">
+        <v>2000</v>
+      </c>
       <c r="K256" t="s">
         <v>377</v>
       </c>
@@ -11496,7 +11622,7 @@
         <v>43009</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>378</v>
       </c>
@@ -11524,6 +11650,9 @@
       <c r="I257">
         <v>98</v>
       </c>
+      <c r="J257">
+        <v>2005</v>
+      </c>
       <c r="K257" t="s">
         <v>379</v>
       </c>
@@ -11531,7 +11660,7 @@
         <v>42736</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>380</v>
       </c>
@@ -11554,13 +11683,16 @@
         <v>1</v>
       </c>
       <c r="H258" s="3">
-        <v>2425</v>
+        <v>95</v>
       </c>
       <c r="I258">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="J258">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="259" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>381</v>
       </c>
@@ -11582,8 +11714,17 @@
       <c r="G259">
         <v>2</v>
       </c>
-    </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H259">
+        <v>246</v>
+      </c>
+      <c r="I259">
+        <v>209</v>
+      </c>
+      <c r="J259">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="260" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>382</v>
       </c>
@@ -11593,14 +11734,29 @@
       <c r="C260" s="2">
         <v>44013</v>
       </c>
+      <c r="D260" t="s">
+        <v>13</v>
+      </c>
+      <c r="E260">
+        <v>2</v>
+      </c>
+      <c r="F260">
+        <v>1</v>
+      </c>
+      <c r="G260">
+        <v>2</v>
+      </c>
       <c r="H260">
         <v>182</v>
       </c>
       <c r="I260">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="J260">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="261" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>383</v>
       </c>
@@ -11626,7 +11782,10 @@
         <v>198</v>
       </c>
       <c r="I261">
-        <v>235</v>
+        <v>217</v>
+      </c>
+      <c r="J261">
+        <v>2003</v>
       </c>
       <c r="K261" t="s">
         <v>384</v>
@@ -11638,7 +11797,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>385</v>
       </c>
@@ -11660,8 +11819,17 @@
       <c r="G262">
         <v>1</v>
       </c>
-    </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H262">
+        <v>84</v>
+      </c>
+      <c r="I262">
+        <v>60</v>
+      </c>
+      <c r="J262">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="263" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>386</v>
       </c>
@@ -11683,8 +11851,17 @@
       <c r="G263">
         <v>1</v>
       </c>
-    </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H263">
+        <v>109</v>
+      </c>
+      <c r="I263">
+        <v>71</v>
+      </c>
+      <c r="J263">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="264" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>387</v>
       </c>
@@ -11694,11 +11871,26 @@
       <c r="C264" s="2">
         <v>44013</v>
       </c>
+      <c r="D264" t="s">
+        <v>13</v>
+      </c>
+      <c r="E264">
+        <v>2</v>
+      </c>
+      <c r="F264">
+        <v>1</v>
+      </c>
+      <c r="G264">
+        <v>1</v>
+      </c>
       <c r="H264" s="3">
-        <v>3723</v>
+        <v>146</v>
       </c>
       <c r="I264">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="J264">
+        <v>1995</v>
       </c>
       <c r="K264" t="s">
         <v>320</v>
@@ -11707,7 +11899,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>388</v>
       </c>
@@ -11735,6 +11927,9 @@
       <c r="I265">
         <v>78</v>
       </c>
+      <c r="J265">
+        <v>2011</v>
+      </c>
       <c r="K265" t="s">
         <v>36</v>
       </c>
@@ -11742,7 +11937,7 @@
         <v>43556</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>389</v>
       </c>
@@ -11770,6 +11965,9 @@
       <c r="I266">
         <v>91</v>
       </c>
+      <c r="J266">
+        <v>2012</v>
+      </c>
       <c r="K266" t="s">
         <v>390</v>
       </c>
@@ -11777,7 +11975,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>391</v>
       </c>
@@ -11799,6 +11997,15 @@
       <c r="G267">
         <v>2</v>
       </c>
+      <c r="H267">
+        <v>237</v>
+      </c>
+      <c r="I267">
+        <v>183</v>
+      </c>
+      <c r="J267">
+        <v>2001</v>
+      </c>
       <c r="K267" t="s">
         <v>181</v>
       </c>
@@ -11806,7 +12013,7 @@
         <v>40817</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>392</v>
       </c>
@@ -11816,11 +12023,29 @@
       <c r="C268" s="2">
         <v>44013</v>
       </c>
+      <c r="D268" t="s">
+        <v>437</v>
+      </c>
+      <c r="E268">
+        <v>0</v>
+      </c>
+      <c r="F268">
+        <v>0</v>
+      </c>
+      <c r="G268">
+        <v>1</v>
+      </c>
       <c r="H268" s="3">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="I268">
+        <v>51</v>
+      </c>
+      <c r="J268">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="269" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>393</v>
       </c>
@@ -11830,8 +12055,26 @@
       <c r="C269" s="2">
         <v>44013</v>
       </c>
+      <c r="D269" t="s">
+        <v>13</v>
+      </c>
+      <c r="E269">
+        <v>2</v>
+      </c>
+      <c r="F269">
+        <v>1</v>
+      </c>
+      <c r="G269">
+        <v>2</v>
+      </c>
       <c r="H269" s="3">
-        <v>3042</v>
+        <v>84</v>
+      </c>
+      <c r="I269">
+        <v>84</v>
+      </c>
+      <c r="J269">
+        <v>1982</v>
       </c>
       <c r="K269" t="s">
         <v>204</v>
@@ -11840,7 +12083,7 @@
         <v>44256</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>394</v>
       </c>
@@ -11850,12 +12093,27 @@
       <c r="C270" s="2">
         <v>44013</v>
       </c>
+      <c r="D270" t="s">
+        <v>13</v>
+      </c>
+      <c r="E270">
+        <v>2</v>
+      </c>
+      <c r="F270">
+        <v>2</v>
+      </c>
+      <c r="G270">
+        <v>2</v>
+      </c>
       <c r="H270">
         <v>115</v>
       </c>
       <c r="I270">
         <v>69</v>
       </c>
+      <c r="J270">
+        <v>2014</v>
+      </c>
       <c r="K270" t="s">
         <v>126</v>
       </c>
@@ -11863,7 +12121,7 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>395</v>
       </c>
@@ -11873,9 +12131,27 @@
       <c r="C271" s="2">
         <v>44013</v>
       </c>
+      <c r="D271" t="s">
+        <v>13</v>
+      </c>
+      <c r="E271">
+        <v>2</v>
+      </c>
+      <c r="F271">
+        <v>1</v>
+      </c>
+      <c r="G271">
+        <v>1</v>
+      </c>
       <c r="H271">
         <v>91</v>
       </c>
+      <c r="I271">
+        <v>70</v>
+      </c>
+      <c r="J271">
+        <v>1999</v>
+      </c>
       <c r="K271" t="s">
         <v>242</v>
       </c>
@@ -11883,7 +12159,7 @@
         <v>43922</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>396</v>
       </c>
@@ -11900,7 +12176,7 @@
         <v>3</v>
       </c>
       <c r="F272">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G272">
         <v>2</v>
@@ -11909,7 +12185,10 @@
         <v>161</v>
       </c>
       <c r="I272">
-        <v>217</v>
+        <v>245</v>
+      </c>
+      <c r="J272">
+        <v>2000</v>
       </c>
       <c r="K272" t="s">
         <v>397</v>
@@ -11918,7 +12197,7 @@
         <v>42675</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>398</v>
       </c>
@@ -11928,14 +12207,29 @@
       <c r="C273" s="2">
         <v>44013</v>
       </c>
+      <c r="D273" t="s">
+        <v>13</v>
+      </c>
+      <c r="E273">
+        <v>3</v>
+      </c>
+      <c r="F273">
+        <v>2</v>
+      </c>
+      <c r="G273">
+        <v>2</v>
+      </c>
       <c r="H273">
         <v>193</v>
       </c>
       <c r="I273">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="J273">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>399</v>
       </c>
@@ -11948,8 +12242,26 @@
       <c r="D274" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E274">
+        <v>2</v>
+      </c>
+      <c r="F274">
+        <v>2</v>
+      </c>
+      <c r="G274">
+        <v>1</v>
+      </c>
+      <c r="H274">
+        <v>119</v>
+      </c>
+      <c r="I274">
+        <v>81</v>
+      </c>
+      <c r="J274">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="275" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>400</v>
       </c>
@@ -11963,7 +12275,7 @@
         <v>17</v>
       </c>
       <c r="E275">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F275">
         <v>3</v>
@@ -11975,10 +12287,13 @@
         <v>285</v>
       </c>
       <c r="I275">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="J275">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="276" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>401</v>
       </c>
@@ -11988,12 +12303,27 @@
       <c r="C276" s="2">
         <v>44013</v>
       </c>
+      <c r="D276" t="s">
+        <v>13</v>
+      </c>
+      <c r="E276">
+        <v>2</v>
+      </c>
+      <c r="F276">
+        <v>1</v>
+      </c>
+      <c r="G276">
+        <v>1</v>
+      </c>
       <c r="H276">
         <v>175</v>
       </c>
       <c r="I276">
         <v>94</v>
       </c>
+      <c r="J276">
+        <v>2000</v>
+      </c>
       <c r="K276" t="s">
         <v>26</v>
       </c>
@@ -12001,7 +12331,7 @@
         <v>41244</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>402</v>
       </c>
@@ -12011,12 +12341,27 @@
       <c r="C277" s="2">
         <v>43983</v>
       </c>
+      <c r="D277" t="s">
+        <v>13</v>
+      </c>
+      <c r="E277">
+        <v>3</v>
+      </c>
+      <c r="F277">
+        <v>2</v>
+      </c>
+      <c r="G277">
+        <v>2</v>
+      </c>
       <c r="H277">
         <v>222</v>
       </c>
       <c r="I277">
         <v>143</v>
       </c>
+      <c r="J277">
+        <v>2005</v>
+      </c>
       <c r="K277" t="s">
         <v>78</v>
       </c>
@@ -12024,7 +12369,7 @@
         <v>42887</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>403</v>
       </c>
@@ -12034,11 +12379,26 @@
       <c r="C278" s="2">
         <v>43983</v>
       </c>
+      <c r="D278" t="s">
+        <v>13</v>
+      </c>
+      <c r="E278">
+        <v>2</v>
+      </c>
+      <c r="F278">
+        <v>1</v>
+      </c>
+      <c r="G278">
+        <v>1</v>
+      </c>
       <c r="H278" s="3">
-        <v>1882</v>
+        <v>101</v>
       </c>
       <c r="I278">
-        <v>80</v>
+        <v>76</v>
+      </c>
+      <c r="J278">
+        <v>2002</v>
       </c>
       <c r="K278" t="s">
         <v>70</v>
@@ -12047,7 +12407,7 @@
         <v>42552</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>404</v>
       </c>
@@ -12057,12 +12417,27 @@
       <c r="C279" s="2">
         <v>43983</v>
       </c>
+      <c r="D279" t="s">
+        <v>13</v>
+      </c>
+      <c r="E279">
+        <v>3</v>
+      </c>
+      <c r="F279">
+        <v>2</v>
+      </c>
+      <c r="G279">
+        <v>2</v>
+      </c>
       <c r="H279">
-        <v>899</v>
+        <v>150</v>
       </c>
       <c r="I279">
         <v>105</v>
       </c>
+      <c r="J279">
+        <v>2006</v>
+      </c>
       <c r="K279" t="s">
         <v>38</v>
       </c>
@@ -12070,7 +12445,7 @@
         <v>43952</v>
       </c>
     </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>405</v>
       </c>
@@ -12095,8 +12470,14 @@
       <c r="H280">
         <v>86</v>
       </c>
-    </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I280">
+        <v>52</v>
+      </c>
+      <c r="J280">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="281" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>406</v>
       </c>
@@ -12119,10 +12500,13 @@
         <v>1</v>
       </c>
       <c r="H281" s="3">
-        <v>1882</v>
+        <v>107</v>
       </c>
       <c r="I281">
-        <v>107</v>
+        <v>76</v>
+      </c>
+      <c r="J281">
+        <v>2002</v>
       </c>
       <c r="K281" t="s">
         <v>204</v>
@@ -12131,7 +12515,7 @@
         <v>40330</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>407</v>
       </c>
@@ -12141,11 +12525,26 @@
       <c r="C282" s="2">
         <v>43983</v>
       </c>
+      <c r="D282" t="s">
+        <v>13</v>
+      </c>
+      <c r="E282">
+        <v>3</v>
+      </c>
+      <c r="F282">
+        <v>2</v>
+      </c>
+      <c r="G282">
+        <v>1</v>
+      </c>
       <c r="H282">
-        <v>137</v>
+        <v>217</v>
       </c>
       <c r="I282">
-        <v>140</v>
+        <v>170</v>
+      </c>
+      <c r="J282">
+        <v>2008</v>
       </c>
       <c r="K282" t="s">
         <v>38</v>
@@ -12154,7 +12553,7 @@
         <v>42856</v>
       </c>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>408</v>
       </c>
@@ -12167,8 +12566,26 @@
       <c r="D283" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E283">
+        <v>2</v>
+      </c>
+      <c r="F283">
+        <v>2</v>
+      </c>
+      <c r="G283">
+        <v>1</v>
+      </c>
+      <c r="H283">
+        <v>130</v>
+      </c>
+      <c r="I283">
+        <v>79</v>
+      </c>
+      <c r="J283">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>409</v>
       </c>
@@ -12196,6 +12613,9 @@
       <c r="I284">
         <v>102</v>
       </c>
+      <c r="J284">
+        <v>2013</v>
+      </c>
       <c r="K284" t="s">
         <v>160</v>
       </c>
@@ -12206,7 +12626,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>410</v>
       </c>
@@ -12234,6 +12654,9 @@
       <c r="I285">
         <v>98</v>
       </c>
+      <c r="J285">
+        <v>2004</v>
+      </c>
       <c r="K285" t="s">
         <v>318</v>
       </c>
@@ -12241,7 +12664,7 @@
         <v>43922</v>
       </c>
     </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>411</v>
       </c>
@@ -12263,8 +12686,17 @@
       <c r="G286">
         <v>2</v>
       </c>
-    </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H286">
+        <v>169</v>
+      </c>
+      <c r="I286">
+        <v>94</v>
+      </c>
+      <c r="J286">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="287" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>412</v>
       </c>
@@ -12287,11 +12719,14 @@
         <v>1</v>
       </c>
       <c r="H287" s="3">
-        <v>1871</v>
+        <v>133</v>
       </c>
       <c r="I287">
         <v>98</v>
       </c>
+      <c r="J287">
+        <v>2005</v>
+      </c>
       <c r="K287" t="s">
         <v>413</v>
       </c>
@@ -12299,7 +12734,7 @@
         <v>43586</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>414</v>
       </c>
@@ -12309,11 +12744,26 @@
       <c r="C288" s="2">
         <v>43983</v>
       </c>
+      <c r="D288" t="s">
+        <v>13</v>
+      </c>
+      <c r="E288">
+        <v>2</v>
+      </c>
+      <c r="F288">
+        <v>2</v>
+      </c>
+      <c r="G288">
+        <v>1</v>
+      </c>
       <c r="H288">
         <v>112</v>
       </c>
       <c r="I288">
-        <v>85</v>
+        <v>87</v>
+      </c>
+      <c r="J288">
+        <v>2002</v>
       </c>
       <c r="K288" t="s">
         <v>291</v>
@@ -12322,7 +12772,7 @@
         <v>43525</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>415</v>
       </c>
@@ -12344,8 +12794,17 @@
       <c r="G289">
         <v>1</v>
       </c>
-    </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H289">
+        <v>81</v>
+      </c>
+      <c r="I289">
+        <v>48</v>
+      </c>
+      <c r="J289">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="290" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>416</v>
       </c>
@@ -12368,11 +12827,14 @@
         <v>2</v>
       </c>
       <c r="H290" s="3">
-        <v>2593</v>
+        <v>123</v>
       </c>
       <c r="I290">
         <v>83</v>
       </c>
+      <c r="J290">
+        <v>2012</v>
+      </c>
       <c r="K290" t="s">
         <v>24</v>
       </c>
@@ -12383,7 +12845,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>417</v>
       </c>
@@ -12405,8 +12867,17 @@
       <c r="G291">
         <v>1</v>
       </c>
-    </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H291">
+        <v>98</v>
+      </c>
+      <c r="I291">
+        <v>70</v>
+      </c>
+      <c r="J291">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="292" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>418</v>
       </c>
@@ -12420,13 +12891,22 @@
         <v>17</v>
       </c>
       <c r="E292">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F292">
         <v>1</v>
       </c>
+      <c r="G292">
+        <v>0</v>
+      </c>
       <c r="H292" s="3">
-        <v>1382</v>
+        <v>75</v>
+      </c>
+      <c r="I292">
+        <v>67</v>
+      </c>
+      <c r="J292">
+        <v>2007</v>
       </c>
       <c r="K292" t="s">
         <v>419</v>
@@ -12435,7 +12915,7 @@
         <v>43070</v>
       </c>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>420</v>
       </c>
@@ -12457,8 +12937,17 @@
       <c r="G293">
         <v>1</v>
       </c>
-    </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H293">
+        <v>118</v>
+      </c>
+      <c r="I293">
+        <v>81</v>
+      </c>
+      <c r="J293">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="294" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>421</v>
       </c>
@@ -12484,7 +12973,10 @@
         <v>168</v>
       </c>
       <c r="I294">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="J294">
+        <v>1990</v>
       </c>
       <c r="K294" t="s">
         <v>63</v>
@@ -12493,7 +12985,7 @@
         <v>43922</v>
       </c>
     </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>422</v>
       </c>
@@ -12521,8 +13013,11 @@
       <c r="I295">
         <v>128</v>
       </c>
-    </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J295">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="296" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>423</v>
       </c>
@@ -12545,11 +13040,14 @@
         <v>1</v>
       </c>
       <c r="H296" s="3">
-        <v>3722</v>
+        <v>85</v>
       </c>
       <c r="I296">
         <v>63</v>
       </c>
+      <c r="J296">
+        <v>2001</v>
+      </c>
       <c r="K296" t="s">
         <v>424</v>
       </c>
@@ -12557,7 +13055,7 @@
         <v>43374</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>425</v>
       </c>
@@ -12580,11 +13078,14 @@
         <v>2</v>
       </c>
       <c r="H297" s="3">
-        <v>3722</v>
+        <v>139</v>
       </c>
       <c r="I297">
         <v>97</v>
       </c>
+      <c r="J297">
+        <v>2001</v>
+      </c>
       <c r="K297" t="s">
         <v>89</v>
       </c>
@@ -12592,7 +13093,7 @@
         <v>43952</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>426</v>
       </c>
@@ -12602,11 +13103,26 @@
       <c r="C298" s="2">
         <v>43952</v>
       </c>
+      <c r="D298" t="s">
+        <v>13</v>
+      </c>
+      <c r="E298">
+        <v>2</v>
+      </c>
+      <c r="F298">
+        <v>2</v>
+      </c>
+      <c r="G298">
+        <v>1</v>
+      </c>
       <c r="H298">
         <v>107</v>
       </c>
       <c r="I298">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="J298">
+        <v>2014</v>
       </c>
       <c r="K298" t="s">
         <v>106</v>
@@ -12615,7 +13131,7 @@
         <v>42856</v>
       </c>
     </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>427</v>
       </c>
@@ -12638,11 +13154,14 @@
         <v>1</v>
       </c>
       <c r="H299" s="3">
-        <v>2201</v>
+        <v>52</v>
       </c>
       <c r="I299">
         <v>52</v>
       </c>
+      <c r="J299">
+        <v>1945</v>
+      </c>
       <c r="K299" t="s">
         <v>242</v>
       </c>
@@ -12650,7 +13169,7 @@
         <v>43160</v>
       </c>
     </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>428</v>
       </c>
@@ -12675,8 +13194,14 @@
       <c r="H300">
         <v>93</v>
       </c>
-    </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I300">
+        <v>61</v>
+      </c>
+      <c r="J300">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="301" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>429</v>
       </c>
@@ -12688,6 +13213,24 @@
       </c>
       <c r="D301" t="s">
         <v>13</v>
+      </c>
+      <c r="E301">
+        <v>1</v>
+      </c>
+      <c r="F301">
+        <v>1</v>
+      </c>
+      <c r="G301">
+        <v>1</v>
+      </c>
+      <c r="H301" s="3">
+        <v>84</v>
+      </c>
+      <c r="I301">
+        <v>48</v>
+      </c>
+      <c r="J301">
+        <v>2019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>